<commit_message>
Line item for deterministic system
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhijit.a.pande\Documents\GitHub\AIML_CAPSTONE_NLP_B_GRP_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D4E2472-E974-460B-8DEE-75FAE73B0D3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9994EA99-6830-4833-B6E6-A457F11B88BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{4CF8E403-727E-4AD3-B9CF-6FEA890FFBCA}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="32">
   <si>
     <t>GIT Master Repo</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>Abhik, Arun, Sayantika</t>
+  </si>
+  <si>
+    <t>Rule based system</t>
   </si>
 </sst>
 </file>
@@ -188,8 +191,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F9D57DB-492C-456C-87C2-037C6E255C39}" name="Table1" displayName="Table1" ref="A1:D19" totalsRowShown="0">
-  <autoFilter ref="A1:D19" xr:uid="{1B2A0889-DA9C-4DCD-B947-E20D792BAF00}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F9D57DB-492C-456C-87C2-037C6E255C39}" name="Table1" displayName="Table1" ref="A1:D20" totalsRowShown="0">
+  <autoFilter ref="A1:D20" xr:uid="{1B2A0889-DA9C-4DCD-B947-E20D792BAF00}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{56084F22-F7BC-423D-8293-830C38D6DB50}" name="Week" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{D02E22E5-A0C3-417C-8499-D527E75F7622}" name="Task"/>
@@ -497,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33F8B665-254D-4F16-81BB-67DB76A18782}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,6 +747,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Data splits and Pickling
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhijit.a.pande\Documents\GitHub\AIML_CAPSTONE_NLP_B_GRP_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9994EA99-6830-4833-B6E6-A457F11B88BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14FB4D5-CB40-4B9D-BA43-AAF06D0DEADA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{4CF8E403-727E-4AD3-B9CF-6FEA890FFBCA}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="33">
   <si>
     <t>GIT Master Repo</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>Rule based system</t>
+  </si>
+  <si>
+    <t>Improvement of visualizations</t>
   </si>
 </sst>
 </file>
@@ -191,8 +194,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F9D57DB-492C-456C-87C2-037C6E255C39}" name="Table1" displayName="Table1" ref="A1:D20" totalsRowShown="0">
-  <autoFilter ref="A1:D20" xr:uid="{1B2A0889-DA9C-4DCD-B947-E20D792BAF00}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F9D57DB-492C-456C-87C2-037C6E255C39}" name="Table1" displayName="Table1" ref="A1:D21" totalsRowShown="0">
+  <autoFilter ref="A1:D21" xr:uid="{1B2A0889-DA9C-4DCD-B947-E20D792BAF00}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{56084F22-F7BC-423D-8293-830C38D6DB50}" name="Week" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{D02E22E5-A0C3-417C-8499-D527E75F7622}" name="Task"/>
@@ -500,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33F8B665-254D-4F16-81BB-67DB76A18782}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,6 +639,9 @@
       <c r="C9" t="s">
         <v>3</v>
       </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -645,7 +651,10 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -680,6 +689,9 @@
       <c r="C13" t="s">
         <v>3</v>
       </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -753,6 +765,17 @@
       </c>
       <c r="B20" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Task updates checked in
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhijit.a.pande\Documents\GitHub\AIML_CAPSTONE_NLP_B_GRP_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98DEDD48-8BFD-4295-AA94-CC2ED20131E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF90D61-EDE8-443A-8B35-E9092D06A41E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{4CF8E403-727E-4AD3-B9CF-6FEA890FFBCA}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="44">
   <si>
     <t>GIT Master Repo</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Word Vocabs and Tokens</t>
   </si>
   <si>
-    <t>Data Augmentation</t>
-  </si>
-  <si>
     <t>Task</t>
   </si>
   <si>
@@ -98,12 +95,6 @@
     <t>Doc2Vec Exploration with Gensim</t>
   </si>
   <si>
-    <t>Translation (follow up with Sumit)</t>
-  </si>
-  <si>
-    <t>Abhik, Abhijit</t>
-  </si>
-  <si>
     <t>Creation of 3 datasets</t>
   </si>
   <si>
@@ -113,9 +104,6 @@
     <t>Feature Engineering (TFIDF Vectorizer, Ngrams, Feature development, weights for balancing)</t>
   </si>
   <si>
-    <t>Hyper parameter tuning</t>
-  </si>
-  <si>
     <t>Machine learning models (SVM, Logistic, XGBoost)</t>
   </si>
   <si>
@@ -125,18 +113,12 @@
     <t>Validate the deliverables against Requirements</t>
   </si>
   <si>
-    <t>Abhik, Arun, Sayantika</t>
-  </si>
-  <si>
     <t>Rule based system</t>
   </si>
   <si>
     <t>Improvement of visualizations</t>
   </si>
   <si>
-    <t>Doubt</t>
-  </si>
-  <si>
     <t>Column1</t>
   </si>
   <si>
@@ -146,9 +128,6 @@
     <t>WEEK3</t>
   </si>
   <si>
-    <t>Move Translation to Goslate</t>
-  </si>
-  <si>
     <t>Resolved. Increase features</t>
   </si>
   <si>
@@ -158,10 +137,34 @@
     <t>Good to have. Not Mandatory</t>
   </si>
   <si>
-    <t>Reduce only to synonyms</t>
-  </si>
-  <si>
     <t>We need to experiment and figure out if Cleaning is impacting this. And try out Goslate</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>Sayantika to update predictions, examples and graphing</t>
+  </si>
+  <si>
+    <t>Need to append graphs and prediction examples</t>
+  </si>
+  <si>
+    <t>We need to connect on Tuesday and put an outline together</t>
+  </si>
+  <si>
+    <t>Use tensor board for visualizations and find hyperparameters</t>
+  </si>
+  <si>
+    <t>Need to graph before and after and provide examples of augmentation and translation</t>
+  </si>
+  <si>
+    <t>Almost Complete</t>
+  </si>
+  <si>
+    <t>Move Translation to Goslate/Improving translations</t>
+  </si>
+  <si>
+    <t>Stratified Training data split</t>
   </si>
 </sst>
 </file>
@@ -230,8 +233,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F9D57DB-492C-456C-87C2-037C6E255C39}" name="Table1" displayName="Table1" ref="A1:F22" totalsRowShown="0">
-  <autoFilter ref="A1:F22" xr:uid="{1B2A0889-DA9C-4DCD-B947-E20D792BAF00}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F9D57DB-492C-456C-87C2-037C6E255C39}" name="Table1" displayName="Table1" ref="A1:F21" totalsRowShown="0">
+  <autoFilter ref="A1:F21" xr:uid="{1B2A0889-DA9C-4DCD-B947-E20D792BAF00}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{56084F22-F7BC-423D-8293-830C38D6DB50}" name="Week" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{D02E22E5-A0C3-417C-8499-D527E75F7622}" name="Task"/>
@@ -541,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33F8B665-254D-4F16-81BB-67DB76A18782}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,27 +560,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>15</v>
-      </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -586,12 +589,12 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -600,12 +603,12 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -614,12 +617,12 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -628,12 +631,12 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -642,18 +645,15 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -662,32 +662,29 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="F8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
@@ -696,165 +693,196 @@
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>35</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
         <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" t="s">
-        <v>40</v>
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>41</v>
+      </c>
+      <c r="F13" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" t="s">
-        <v>33</v>
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
       </c>
       <c r="F14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" t="s">
-        <v>33</v>
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>26</v>
-      </c>
-      <c r="C16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>24</v>
       </c>
       <c r="C17" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" t="s">
-        <v>37</v>
+      <c r="D21" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated with Graphs and Examples for augmentation and Language translation
Tweaked augmentation also. Might need to rerun it and maybe it will improve accuracy
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhijit.a.pande\Documents\GitHub\AIML_CAPSTONE_NLP_B_GRP_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF90D61-EDE8-443A-8B35-E9092D06A41E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F523F9-E0A7-4023-9D01-11B5022352AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{4CF8E403-727E-4AD3-B9CF-6FEA890FFBCA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4CF8E403-727E-4AD3-B9CF-6FEA890FFBCA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -234,7 +234,6 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F9D57DB-492C-456C-87C2-037C6E255C39}" name="Table1" displayName="Table1" ref="A1:F21" totalsRowShown="0">
-  <autoFilter ref="A1:F21" xr:uid="{1B2A0889-DA9C-4DCD-B947-E20D792BAF00}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{56084F22-F7BC-423D-8293-830C38D6DB50}" name="Week" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{D02E22E5-A0C3-417C-8499-D527E75F7622}" name="Task"/>
@@ -547,7 +546,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,7 +675,7 @@
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="F8" t="s">
         <v>40</v>
@@ -809,7 +808,7 @@
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -882,7 +881,7 @@
         <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated report with sections 2,3,4
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhijit.a.pande\Documents\GitHub\AIML_CAPSTONE_NLP_B_GRP_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F523F9-E0A7-4023-9D01-11B5022352AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3966079D-0995-481A-AC6E-46A3A3E603E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4CF8E403-727E-4AD3-B9CF-6FEA890FFBCA}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="45">
   <si>
     <t>GIT Master Repo</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>Stratified Training data split</t>
+  </si>
+  <si>
+    <t>WEEK 3</t>
   </si>
 </sst>
 </file>
@@ -234,6 +237,21 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F9D57DB-492C-456C-87C2-037C6E255C39}" name="Table1" displayName="Table1" ref="A1:F21" totalsRowShown="0">
+  <autoFilter ref="A1:F21" xr:uid="{6B2D9500-BCDD-4273-9860-C80BE7AF3AE6}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Almost Complete"/>
+        <filter val="Pending"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="5">
+      <filters blank="1">
+        <filter val="Need to append graphs and prediction examples"/>
+        <filter val="Sayantika to update predictions, examples and graphing"/>
+        <filter val="We need to connect on Tuesday and put an outline together"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{56084F22-F7BC-423D-8293-830C38D6DB50}" name="Week" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{D02E22E5-A0C3-417C-8499-D527E75F7622}" name="Task"/>
@@ -546,7 +564,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,7 +595,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -591,7 +609,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -605,7 +623,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -619,7 +637,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -633,7 +651,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -650,7 +668,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -664,7 +682,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -681,7 +699,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -695,7 +713,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -715,7 +733,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -729,7 +747,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
@@ -797,7 +815,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -839,9 +857,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s">
         <v>42</v>
@@ -858,7 +876,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B20" t="s">
         <v>39</v>
@@ -870,7 +888,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Added task list for week4
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhijit.a.pande\Documents\GitHub\AIML_CAPSTONE_NLP_B_GRP_4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abhik Kar\OneDrive\Documents\GitHub\AIML_CAPSTONE_NLP_B_GRP_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3966079D-0995-481A-AC6E-46A3A3E603E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4CF8E403-727E-4AD3-B9CF-6FEA890FFBCA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="54">
   <si>
     <t>GIT Master Repo</t>
   </si>
@@ -168,12 +167,39 @@
   </si>
   <si>
     <t>WEEK 3</t>
+  </si>
+  <si>
+    <t>Add New Machine Learning Techniques: LightGBM, CatBoost, Random forest With Random and Grid search for all of these</t>
+  </si>
+  <si>
+    <t>SVC try with different kernel in grid search</t>
+  </si>
+  <si>
+    <t>In the accuracy score table also add scores from data without augmentation</t>
+  </si>
+  <si>
+    <t>Model interpretation - Lime and other packages</t>
+  </si>
+  <si>
+    <t>Add Embedding projection using Tensor board</t>
+  </si>
+  <si>
+    <t>Add visualization for train, test data and show all groups are present in both set</t>
+  </si>
+  <si>
+    <t>Deep learning hypeparameter tuning using packages</t>
+  </si>
+  <si>
+    <t>WEEK 4</t>
+  </si>
+  <si>
+    <t>Clustering of data and visualization: Topic Modeling (use LDAPyviz), Document clustering</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -209,10 +235,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -236,8 +265,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F9D57DB-492C-456C-87C2-037C6E255C39}" name="Table1" displayName="Table1" ref="A1:F21" totalsRowShown="0">
-  <autoFilter ref="A1:F21" xr:uid="{6B2D9500-BCDD-4273-9860-C80BE7AF3AE6}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F29" totalsRowShown="0">
+  <autoFilter ref="A1:F29">
     <filterColumn colId="3">
       <filters>
         <filter val="Almost Complete"/>
@@ -253,12 +282,12 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{56084F22-F7BC-423D-8293-830C38D6DB50}" name="Week" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{D02E22E5-A0C3-417C-8499-D527E75F7622}" name="Task"/>
-    <tableColumn id="3" xr3:uid="{FF2D9910-2001-4280-84CA-9EB3B2B3A020}" name="Owner"/>
-    <tableColumn id="4" xr3:uid="{86D1D916-33C5-4D25-8463-EF9F0B0700D5}" name="Status"/>
-    <tableColumn id="5" xr3:uid="{F5833AAE-446C-437C-9C8E-47A0E2BBA3B3}" name="Column1"/>
-    <tableColumn id="6" xr3:uid="{C7CA6A14-1991-4296-8051-071BBA696ABA}" name="Column2"/>
+    <tableColumn id="1" name="Week" dataDxfId="0"/>
+    <tableColumn id="2" name="Task"/>
+    <tableColumn id="3" name="Owner"/>
+    <tableColumn id="4" name="Status"/>
+    <tableColumn id="5" name="Column1"/>
+    <tableColumn id="6" name="Column2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -560,11 +589,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33F8B665-254D-4F16-81BB-67DB76A18782}">
-  <dimension ref="A1:F21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,11 +931,124 @@
         <v>15</v>
       </c>
     </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final models and Code
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,17 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhijit.a.pande\Documents\GitHub\AIML_CAPSTONE_NLP_B_GRP_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F627F2DD-F1C1-4952-BFC6-CB606A6FD62A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FED539B-0BC9-4C1D-ABDC-F1F80B81E707}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -278,6 +286,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F29" totalsRowShown="0">
+  <autoFilter ref="A1:F29" xr:uid="{EE06DA43-9E24-46F2-BC93-47EBE67A5C6D}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Week" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Task"/>
@@ -590,7 +599,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,7 +875,7 @@
         <v>3</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>50</v>
@@ -883,7 +892,7 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -914,7 +923,7 @@
         <v>3</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -984,7 +993,7 @@
         <v>7</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -998,7 +1007,7 @@
         <v>2</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1043,7 +1052,7 @@
         <v>7</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>